<commit_message>
so it turns out that three-dots and semi-colons can't be parsed by the squib csv file parser. Ithink there's a way around it but I'm not too invested in like, making a PR to their github or whatever.Reason this came up is I added columns for comments.... ideally we can find a way to work around this, maybe by programmatically removing those columns?
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_1_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_1_CC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AD4515-C094-45DD-8035-A236BF91976D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EF2319-34E2-4457-B0E1-A4679DE34186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="26370" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,9 +419,6 @@
     <t>Reduce this attack value by X. If damage is still dealt then deal X twice to damage to that target</t>
   </si>
   <si>
-    <t>Wager is poor against enemies with high defense, no need to change it?</t>
-  </si>
-  <si>
     <t>Appear Aggressive</t>
   </si>
   <si>
@@ -933,13 +930,6 @@
     <t>Recalibrating/Reorient Focus/Refocus/Redirect Attention/Reprioritize</t>
   </si>
   <si>
-    <t>moving a single token, even it this card returns to hand, feels exceptionally weak… maybe move up to 2 tokens?</t>
-  </si>
-  <si>
-    <t>like destiny swap, but requires succeed influence, and reduces by x instead of Min…
-maybe needs to last more rounds? Acutally what I like better, make all their rolls reduce by X instead of just the first</t>
-  </si>
-  <si>
     <t>add X to attack value if marked, then remove mark from target</t>
   </si>
   <si>
@@ -967,9 +957,6 @@
     <t>pinpoint punishment</t>
   </si>
   <si>
-    <t>This feels too boring. It's the kind of thing I'd always want to be playing if I had the choice, it's just a good attack. Doesn't relate to pinpoint at all, because there's not cost to try and focus, it feels like making a called show but without any challenge... maybe contesdted influence to get the extra damage?</t>
-  </si>
-  <si>
     <t>add level to damage</t>
   </si>
   <si>
@@ -1174,9 +1161,6 @@
     <t>gain discarded cards * 5 in movement</t>
   </si>
   <si>
-    <t>requires moving after this attack, otherwise is useless… weak?</t>
-  </si>
-  <si>
     <t>composed</t>
   </si>
   <si>
@@ -1223,6 +1207,22 @@
   </si>
   <si>
     <t>must get attacked in round following attack, must defend against all damage, discard</t>
+  </si>
+  <si>
+    <t>This feels too boring-It's the kind of thing I'd always want to be playing if I had the choice--it's just a good attack__Doesn't relate to pinpoint at all--because there's not cost to try and focus--it feels like making a called shot but without any challenge___maybe contested influence to get the extra damage</t>
+  </si>
+  <si>
+    <t>moving a single token--even if this card returns to hand--feels exceptionally weak__maybe move up to 2 tokens</t>
+  </si>
+  <si>
+    <t>like destiny swap--but requires succeed influence--and reduces by x instead of Mn__
+maybe needs to last more rounds__Acutally what I like better--make all their rolls reduce by X instead of just the first</t>
+  </si>
+  <si>
+    <t>requires moving after this attack--otherwise is useless___weak</t>
+  </si>
+  <si>
+    <t>Wager is poor against enemies with high defense--no need to change it maybe</t>
   </si>
 </sst>
 </file>
@@ -2079,8 +2079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="J16" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2133,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>17</v>
@@ -2169,7 +2169,7 @@
         <v>15</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>17</v>
@@ -2198,16 +2198,16 @@
         <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>25</v>
@@ -2237,10 +2237,10 @@
         <v>32</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -2260,16 +2260,16 @@
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>37</v>
@@ -2287,7 +2287,7 @@
         <v>23</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>24</v>
@@ -2299,10 +2299,10 @@
         <v>32</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -2322,16 +2322,16 @@
         <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>42</v>
@@ -2358,10 +2358,10 @@
         <v>32</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="105" x14ac:dyDescent="0.25">
@@ -2384,10 +2384,10 @@
         <v>48</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>301</v>
+        <v>394</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>49</v>
@@ -2417,10 +2417,10 @@
         <v>32</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>312</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2446,10 +2446,10 @@
         <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>54</v>
@@ -2479,7 +2479,7 @@
         <v>32</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="120" x14ac:dyDescent="0.25">
@@ -2505,10 +2505,10 @@
         <v>48</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>302</v>
+        <v>395</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>62</v>
@@ -2538,7 +2538,7 @@
         <v>32</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2558,16 +2558,16 @@
         <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>67</v>
@@ -2597,7 +2597,7 @@
         <v>32</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="75" x14ac:dyDescent="0.25">
@@ -2623,10 +2623,10 @@
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>72</v>
@@ -2644,7 +2644,7 @@
         <v>44</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>30</v>
@@ -2656,7 +2656,7 @@
         <v>32</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2682,10 +2682,10 @@
         <v>30</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>76</v>
@@ -2715,7 +2715,7 @@
         <v>32</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -3015,7 +3015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>106</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>111</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>116</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>122</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>126</v>
       </c>
@@ -3264,13 +3264,13 @@
       <c r="S21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="T21" s="1" t="s">
+      <c r="U21" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>39</v>
@@ -3285,13 +3285,13 @@
         <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>39</v>
@@ -3306,7 +3306,7 @@
         <v>23</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>24</v>
@@ -3318,9 +3318,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>97</v>
@@ -3329,19 +3329,19 @@
         <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>97</v>
@@ -3356,7 +3356,7 @@
         <v>23</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>30</v>
@@ -3368,9 +3368,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>43</v>
@@ -3379,19 +3379,19 @@
         <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>43</v>
@@ -3403,7 +3403,7 @@
         <v>44</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>30</v>
@@ -3415,9 +3415,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>39</v>
@@ -3432,13 +3432,13 @@
         <v>41</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>43</v>
@@ -3453,7 +3453,7 @@
         <v>44</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>24</v>
@@ -3465,9 +3465,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>43</v>
@@ -3476,19 +3476,19 @@
         <v>35</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>43</v>
@@ -3497,13 +3497,13 @@
         <v>35</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>24</v>
@@ -3515,9 +3515,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>39</v>
@@ -3532,13 +3532,13 @@
         <v>41</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>39</v>
@@ -3553,7 +3553,7 @@
         <v>41</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>24</v>
@@ -3565,9 +3565,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>39</v>
@@ -3582,13 +3582,13 @@
         <v>41</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>39</v>
@@ -3603,7 +3603,7 @@
         <v>41</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>24</v>
@@ -3615,30 +3615,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>97</v>
@@ -3647,13 +3647,13 @@
         <v>35</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>30</v>
@@ -3665,9 +3665,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>43</v>
@@ -3676,19 +3676,19 @@
         <v>56</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>39</v>
@@ -3703,7 +3703,7 @@
         <v>41</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>48</v>
@@ -3715,9 +3715,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>39</v>
@@ -3732,13 +3732,13 @@
         <v>41</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>39</v>
@@ -3753,7 +3753,7 @@
         <v>23</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q31" s="1" t="s">
         <v>24</v>
@@ -3765,9 +3765,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>39</v>
@@ -3782,13 +3782,13 @@
         <v>41</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>39</v>
@@ -3803,7 +3803,7 @@
         <v>41</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q32" s="1" t="s">
         <v>24</v>
@@ -3817,7 +3817,7 @@
     </row>
     <row r="33" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>39</v>
@@ -3832,13 +3832,13 @@
         <v>41</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>39</v>
@@ -3850,7 +3850,7 @@
         <v>23</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>30</v>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="34" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>39</v>
@@ -3879,13 +3879,13 @@
         <v>23</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>39</v>
@@ -3900,7 +3900,7 @@
         <v>41</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>30</v>
@@ -3914,10 +3914,10 @@
     </row>
     <row r="35" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>35</v>
@@ -3926,16 +3926,16 @@
         <v>23</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>56</v>
@@ -3944,7 +3944,7 @@
         <v>23</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>30</v>
@@ -3958,7 +3958,7 @@
     </row>
     <row r="36" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>39</v>
@@ -3973,13 +3973,13 @@
         <v>23</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>43</v>
@@ -3991,7 +3991,7 @@
         <v>44</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>30</v>
@@ -4005,7 +4005,7 @@
     </row>
     <row r="37" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>43</v>
@@ -4017,13 +4017,13 @@
         <v>44</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>97</v>
@@ -4032,13 +4032,13 @@
         <v>56</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>24</v>
@@ -4052,7 +4052,7 @@
     </row>
     <row r="38" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>39</v>
@@ -4067,13 +4067,13 @@
         <v>41</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>55</v>
@@ -4082,13 +4082,13 @@
         <v>70</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>30</v>
@@ -4102,28 +4102,28 @@
     </row>
     <row r="39" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>43</v>
@@ -4138,7 +4138,7 @@
         <v>44</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>24</v>
@@ -4152,7 +4152,7 @@
     </row>
     <row r="40" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>97</v>
@@ -4161,19 +4161,19 @@
         <v>70</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>39</v>
@@ -4188,7 +4188,7 @@
         <v>23</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q40" s="1" t="s">
         <v>24</v>
@@ -4202,7 +4202,7 @@
     </row>
     <row r="41" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>39</v>
@@ -4217,13 +4217,13 @@
         <v>41</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>39</v>
@@ -4238,7 +4238,7 @@
         <v>41</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q41" s="1" t="s">
         <v>48</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="42" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>39</v>
@@ -4267,31 +4267,31 @@
         <v>41</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="K42" s="2" t="s">
+      <c r="L42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N42" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="O42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="Q42" s="1" t="s">
         <v>48</v>
@@ -4305,7 +4305,7 @@
     </row>
     <row r="43" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>39</v>
@@ -4320,13 +4320,13 @@
         <v>41</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>39</v>
@@ -4341,7 +4341,7 @@
         <v>41</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q43" s="1" t="s">
         <v>24</v>
@@ -4355,7 +4355,7 @@
     </row>
     <row r="44" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>39</v>
@@ -4370,13 +4370,13 @@
         <v>41</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>39</v>
@@ -4391,7 +4391,7 @@
         <v>41</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q44" s="1" t="s">
         <v>24</v>
@@ -4405,7 +4405,7 @@
     </row>
     <row r="45" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>39</v>
@@ -4420,13 +4420,13 @@
         <v>41</v>
       </c>
       <c r="F45" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K45" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>39</v>
@@ -4441,7 +4441,7 @@
         <v>41</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>30</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="46" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>39</v>
@@ -4470,13 +4470,13 @@
         <v>41</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>43</v>
@@ -4491,7 +4491,7 @@
         <v>44</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q46" s="1" t="s">
         <v>30</v>
@@ -4505,7 +4505,7 @@
     </row>
     <row r="47" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>97</v>
@@ -4514,19 +4514,19 @@
         <v>35</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K47" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>39</v>
@@ -4541,7 +4541,7 @@
         <v>23</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q47" s="1" t="s">
         <v>48</v>
@@ -4555,7 +4555,7 @@
     </row>
     <row r="48" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>43</v>
@@ -4564,19 +4564,19 @@
         <v>70</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>39</v>
@@ -4591,7 +4591,7 @@
         <v>23</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q48" s="1" t="s">
         <v>30</v>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="49" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>43</v>
@@ -4620,13 +4620,13 @@
         <v>44</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>43</v>
@@ -4641,7 +4641,7 @@
         <v>44</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q49" s="1" t="s">
         <v>30</v>
@@ -4655,7 +4655,7 @@
     </row>
     <row r="50" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>43</v>
@@ -4664,19 +4664,19 @@
         <v>70</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>39</v>
@@ -4691,7 +4691,7 @@
         <v>23</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q50" s="1" t="s">
         <v>30</v>
@@ -4705,7 +4705,7 @@
     </row>
     <row r="51" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>43</v>
@@ -4720,13 +4720,13 @@
         <v>44</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>39</v>
@@ -4735,13 +4735,13 @@
         <v>70</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O51" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q51" s="1" t="s">
         <v>24</v>
@@ -4755,7 +4755,7 @@
     </row>
     <row r="52" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>39</v>
@@ -4770,13 +4770,13 @@
         <v>23</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K52" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>97</v>
@@ -4791,7 +4791,7 @@
         <v>44</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>24</v>
@@ -4805,7 +4805,7 @@
     </row>
     <row r="53" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>97</v>
@@ -4814,19 +4814,19 @@
         <v>70</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K53" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>97</v>
@@ -4835,13 +4835,13 @@
         <v>21</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O53" s="1" t="s">
         <v>44</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q53" s="1" t="s">
         <v>24</v>
@@ -4855,28 +4855,28 @@
     </row>
     <row r="54" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K54" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>39</v>
@@ -4891,7 +4891,7 @@
         <v>41</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>24</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="55" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>34</v>
@@ -4914,19 +4914,19 @@
         <v>35</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F55" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K55" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>284</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>34</v>
@@ -4935,13 +4935,13 @@
         <v>35</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O55" s="1" t="s">
         <v>44</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>30</v>
@@ -4976,24 +4976,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5001,10 +5001,10 @@
         <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5012,109 +5012,109 @@
         <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C8" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B9" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C9" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B10" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C10" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B11" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C11" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B12" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C12" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B14" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B15" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="C15" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5122,73 +5122,73 @@
         <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C17" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B18" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C18" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B21" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C21" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B22" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C22" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C23" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C24" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5196,65 +5196,65 @@
         <v>111</v>
       </c>
       <c r="B26" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C26" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B27" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C27" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B28" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C28" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B29" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C29" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B30" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C30" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B32" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C32" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5262,101 +5262,101 @@
         <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C33" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B34" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C34" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B36" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C36" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C37" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B38" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C38" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C39" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C40" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B41" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C41" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B42" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C42" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -5364,21 +5364,21 @@
         <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C43" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B44" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C44" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -5386,21 +5386,21 @@
         <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C45" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B46" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C46" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -5408,76 +5408,76 @@
         <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C48" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B49" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C49" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B50" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C50" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B51" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C51" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B53" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C53" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B54" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C54" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B55" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C55" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating level 1 cards to use new level points, and with level 2. also adding another perception focused card
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_1_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_1_CC.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EF2319-34E2-4457-B0E1-A4679DE34186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD53D269-DE01-4E57-98FC-688275FB87AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="26370" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Level 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="397">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Exhaust</t>
   </si>
   <si>
-    <t>1 Skill Point</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
   </si>
   <si>
     <t>Add X to attack value</t>
-  </si>
-  <si>
-    <t>1 Health</t>
   </si>
   <si>
     <t>Flip</t>
@@ -1223,13 +1217,16 @@
   </si>
   <si>
     <t>Wager is poor against enemies with high defense--no need to change it maybe</t>
+  </si>
+  <si>
+    <t>2 Level Points</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1360,6 +1357,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2079,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J16" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" topLeftCell="J51" workbookViewId="0">
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2136,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>17</v>
@@ -2169,7 +2172,7 @@
         <v>15</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>17</v>
@@ -2198,16 +2201,16 @@
         <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>25</v>
@@ -2231,54 +2234,54 @@
         <v>30</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="T2" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>28</v>
@@ -2287,2673 +2290,2674 @@
         <v>23</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="T3" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="T4" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="Q5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="T7" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="L8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="Q8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="T8" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="T9" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="L12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="Q12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="L13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="2" t="s">
+      <c r="P13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="Q13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="L14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="Q14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R15" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R16" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="L17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="2" t="s">
+      <c r="P17" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="L18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="2" t="s">
+      <c r="P18" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R18" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S18" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="G19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="L19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" s="2" t="s">
+      <c r="O19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="Q19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R19" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S19" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R20" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S20" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="G21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="L21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" s="2" t="s">
+      <c r="O21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="Q21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R22" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R23" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S23" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="P24" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R24" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S24" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="L25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P25" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="Q25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R25" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N26" s="1" t="s">
+      <c r="Q26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P26" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="Q26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R26" s="1" t="s">
+      <c r="G27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S27" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O28" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="P28" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R28" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S28" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="G29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="L29" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="G30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="L30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="L31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Q31" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R31" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S31" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="L32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="Q32" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R33" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S33" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S33" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P34" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R35" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S35" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S35" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P36" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R36" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S36" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S36" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" s="1" t="s">
+      <c r="L37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N37" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R37" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S37" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S37" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" s="1" t="s">
+      <c r="L38" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N38" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P39" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="Q39" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R39" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S39" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S39" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Q40" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R40" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S40" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S40" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="L41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P41" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="Q41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="L42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="O42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I42" s="1" t="s">
+      <c r="P42" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R42" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="K42" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="S42" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="L43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" s="1" t="s">
+      <c r="P43" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="Q43" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R43" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S43" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S43" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="1" t="s">
+      <c r="L44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P44" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="Q44" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K45" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="L45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="P45" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R45" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S45" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S45" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O46" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M46" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="P46" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="Q46" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R46" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S46" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S46" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O47" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R47" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S47" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S47" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O48" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Q48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R48" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S48" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S48" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M49" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O49" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="P49" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="Q49" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R49" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S49" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S49" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O50" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="Q50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R50" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S50" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S50" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K51" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P51" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="Q51" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P52" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="Q52" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R52" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S52" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S52" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>24</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>21</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="Q53" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R53" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S53" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="S53" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="G54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N54" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F54" s="1" t="s">
+      <c r="O54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P54" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N54" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P54" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="Q54" s="1" t="s">
         <v>24</v>
       </c>
       <c r="R54" s="1" t="s">
-        <v>51</v>
+        <v>396</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K55" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F55" s="1" t="s">
+      <c r="L55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P55" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N55" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="O55" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P55" s="1" t="s">
-        <v>284</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>30</v>
       </c>
       <c r="R55" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="S55" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S55" s="1" t="s">
-        <v>32</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -4976,508 +4980,508 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" t="s">
         <v>304</v>
-      </c>
-      <c r="B1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" t="s">
         <v>348</v>
       </c>
-      <c r="B2" t="s">
-        <v>350</v>
-      </c>
       <c r="C2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B6" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" t="s">
         <v>342</v>
-      </c>
-      <c r="B6" t="s">
-        <v>343</v>
-      </c>
-      <c r="C6" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C9" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C11" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14" t="s">
         <v>305</v>
-      </c>
-      <c r="B14" t="s">
-        <v>327</v>
-      </c>
-      <c r="C14" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B15" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C17" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C18" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B20" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>343</v>
+      </c>
+      <c r="B21" t="s">
+        <v>344</v>
+      </c>
+      <c r="C21" t="s">
         <v>345</v>
-      </c>
-      <c r="B21" t="s">
-        <v>346</v>
-      </c>
-      <c r="C21" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B22" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C22" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C23" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C24" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C26" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B27" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C27" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B28" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B29" t="s">
+        <v>388</v>
+      </c>
+      <c r="C29" t="s">
         <v>390</v>
-      </c>
-      <c r="C29" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B30" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C30" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B32" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C32" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C33" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B34" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C34" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B36" t="s">
+        <v>349</v>
+      </c>
+      <c r="C36" t="s">
         <v>351</v>
-      </c>
-      <c r="C36" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C37" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B38" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C39" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C40" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C41" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B42" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C42" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C43" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B44" t="s">
+        <v>353</v>
+      </c>
+      <c r="C44" t="s">
         <v>355</v>
-      </c>
-      <c r="C44" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C45" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B46" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C46" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C48" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B49" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C49" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>317</v>
+      </c>
+      <c r="B50" t="s">
+        <v>318</v>
+      </c>
+      <c r="C50" t="s">
         <v>319</v>
-      </c>
-      <c r="B50" t="s">
-        <v>320</v>
-      </c>
-      <c r="C50" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B51" t="s">
+        <v>354</v>
+      </c>
+      <c r="C51" t="s">
         <v>356</v>
-      </c>
-      <c r="C51" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B53" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C53" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B54" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C54" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B55" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C55" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removing ..., which apparently breaks squib
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_1_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_1_CC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257674D4-5304-4436-9D47-E35B30601730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11167F8-2EF4-4D29-932D-1E0326DBD69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="409">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -862,11 +862,6 @@
     <t>X are targeted, healed by Y amount. Exhaust a card.</t>
   </si>
   <si>
-    <t>Summon either: 
-Large Plant [all die=your influence die, range 5ft, health=X, no movement] 
-Medium Creature [attack die=2 * X, defense=X, range 5ft, health=Y, movement=20 ft]</t>
-  </si>
-  <si>
     <t>Empowered Fertilizer/Quick Maturation/Abridged Development/Quick, Harvest!</t>
   </si>
   <si>
@@ -1210,9 +1205,6 @@
   </si>
   <si>
     <t>Refresh/Recharge</t>
-  </si>
-  <si>
-    <t>we should probably create a shorthand for summoning rules… if the doc describes the format, like how it describes the discard/exhaust/handedness, we could 1) get some consistency and 2) keep these rules concise</t>
   </si>
   <si>
     <t>X = up to Level</t>
@@ -1253,6 +1245,15 @@
   <si>
     <t>like destiny swap, but requires succeed influence, and reduces by x instead of Mn.
 maybe needs to last more rounds. Acutally what I like better, make all their rolls reduce by X instead of just the first</t>
+  </si>
+  <si>
+    <t>Summon either:     Large Plant [all die=your influence die, range 5ft, health=X, no movement]     Medium Creature [attack die=2 * X, defense=X, range 5ft, health=Y, movement=20 ft]</t>
+  </si>
+  <si>
+    <t>we should probably create a shorthand for summoning rule. if the doc describes the format, like how it describes the discard/exhaust/handedness, we could get some consistency and keep these rules concise</t>
+  </si>
+  <si>
+    <t>character's that are bad for squib: new lines,the dot dot dot single character,</t>
   </si>
 </sst>
 </file>
@@ -2113,11 +2114,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2147,7 +2148,7 @@
     <col min="23" max="16384" width="22.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2215,7 +2216,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -2238,10 +2239,10 @@
         <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>23</v>
@@ -2265,19 +2266,22 @@
         <v>28</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T2" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="W2" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -2294,16 +2298,16 @@
         <v>92</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>34</v>
@@ -2327,19 +2331,19 @@
         <v>22</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
@@ -2353,19 +2357,19 @@
         <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>38</v>
@@ -2377,7 +2381,7 @@
         <v>32</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>40</v>
@@ -2386,19 +2390,19 @@
         <v>28</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -2418,10 +2422,10 @@
         <v>43</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>44</v>
@@ -2436,7 +2440,7 @@
         <v>68</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>45</v>
@@ -2445,19 +2449,19 @@
         <v>22</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
@@ -2471,7 +2475,7 @@
         <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>47</v>
@@ -2480,10 +2484,10 @@
         <v>22</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>48</v>
@@ -2498,7 +2502,7 @@
         <v>51</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>52</v>
@@ -2507,19 +2511,19 @@
         <v>28</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -2542,10 +2546,10 @@
         <v>43</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>56</v>
@@ -2569,19 +2573,19 @@
         <v>43</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>59</v>
       </c>
@@ -2595,19 +2599,19 @@
         <v>60</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>61</v>
@@ -2622,7 +2626,7 @@
         <v>51</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>62</v>
@@ -2631,19 +2635,19 @@
         <v>22</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>63</v>
       </c>
@@ -2663,10 +2667,10 @@
         <v>22</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>66</v>
@@ -2681,28 +2685,28 @@
         <v>26</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>278</v>
+        <v>406</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>67</v>
       </c>
@@ -2716,7 +2720,7 @@
         <v>68</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>69</v>
@@ -2725,10 +2729,10 @@
         <v>28</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>70</v>
@@ -2740,10 +2744,10 @@
         <v>50</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>71</v>
@@ -2752,19 +2756,19 @@
         <v>22</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>72</v>
       </c>
@@ -2787,10 +2791,10 @@
         <v>28</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>74</v>
@@ -2811,16 +2815,16 @@
         <v>43</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>76</v>
       </c>
@@ -2834,7 +2838,7 @@
         <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>77</v>
@@ -2843,10 +2847,10 @@
         <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>78</v>
@@ -2861,25 +2865,25 @@
         <v>51</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>79</v>
       </c>
@@ -2893,7 +2897,7 @@
         <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>80</v>
@@ -2902,10 +2906,10 @@
         <v>22</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>81</v>
@@ -2920,7 +2924,7 @@
         <v>82</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>83</v>
@@ -2929,16 +2933,16 @@
         <v>22</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>84</v>
       </c>
@@ -2952,7 +2956,7 @@
         <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>85</v>
@@ -2973,7 +2977,7 @@
         <v>68</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>87</v>
@@ -2982,16 +2986,16 @@
         <v>22</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>88</v>
       </c>
@@ -3005,7 +3009,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>90</v>
@@ -3035,13 +3039,13 @@
         <v>43</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>94</v>
       </c>
@@ -3085,7 +3089,7 @@
         <v>28</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>29</v>
@@ -3105,7 +3109,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>99</v>
@@ -3126,7 +3130,7 @@
         <v>101</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>102</v>
@@ -3135,7 +3139,7 @@
         <v>28</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>29</v>
@@ -3155,7 +3159,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>104</v>
@@ -3176,7 +3180,7 @@
         <v>106</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>107</v>
@@ -3185,7 +3189,7 @@
         <v>28</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>29</v>
@@ -3205,7 +3209,7 @@
         <v>109</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>110</v>
@@ -3226,7 +3230,7 @@
         <v>112</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>113</v>
@@ -3235,7 +3239,7 @@
         <v>22</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>29</v>
@@ -3264,7 +3268,7 @@
         <v>28</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>116</v>
@@ -3288,7 +3292,7 @@
         <v>22</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>29</v>
@@ -3308,7 +3312,7 @@
         <v>119</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>120</v>
@@ -3329,7 +3333,7 @@
         <v>122</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>123</v>
@@ -3338,13 +3342,13 @@
         <v>22</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -3391,7 +3395,7 @@
         <v>22</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>29</v>
@@ -3441,7 +3445,7 @@
         <v>28</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>29</v>
@@ -3461,7 +3465,7 @@
         <v>134</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>135</v>
@@ -3479,7 +3483,7 @@
         <v>32</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>137</v>
@@ -3488,7 +3492,7 @@
         <v>28</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>29</v>
@@ -3508,7 +3512,7 @@
         <v>68</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>139</v>
@@ -3526,7 +3530,7 @@
         <v>32</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>141</v>
@@ -3535,7 +3539,7 @@
         <v>22</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>29</v>
@@ -3555,7 +3559,7 @@
         <v>143</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>144</v>
@@ -3576,7 +3580,7 @@
         <v>146</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>147</v>
@@ -3585,7 +3589,7 @@
         <v>22</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S26" s="1" t="s">
         <v>29</v>
@@ -3605,7 +3609,7 @@
         <v>37</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>149</v>
@@ -3626,7 +3630,7 @@
         <v>37</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>151</v>
@@ -3635,7 +3639,7 @@
         <v>22</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>29</v>
@@ -3655,7 +3659,7 @@
         <v>112</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>153</v>
@@ -3676,7 +3680,7 @@
         <v>37</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>155</v>
@@ -3685,7 +3689,7 @@
         <v>22</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S28" s="1" t="s">
         <v>29</v>
@@ -3705,7 +3709,7 @@
         <v>157</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>158</v>
@@ -3735,7 +3739,7 @@
         <v>28</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S29" s="1" t="s">
         <v>29</v>
@@ -3755,7 +3759,7 @@
         <v>33</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>162</v>
@@ -3764,7 +3768,7 @@
         <v>22</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>163</v>
@@ -3779,22 +3783,22 @@
         <v>68</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>43</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="60" x14ac:dyDescent="0.25">
@@ -3811,7 +3815,7 @@
         <v>37</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>165</v>
@@ -3841,7 +3845,7 @@
         <v>22</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S31" s="1" t="s">
         <v>29</v>
@@ -3861,7 +3865,7 @@
         <v>37</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>169</v>
@@ -3882,7 +3886,7 @@
         <v>37</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P32" s="1" t="s">
         <v>171</v>
@@ -3891,7 +3895,7 @@
         <v>22</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S32" s="1" t="s">
         <v>29</v>
@@ -3911,7 +3915,7 @@
         <v>122</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>173</v>
@@ -3938,7 +3942,7 @@
         <v>28</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S33" s="1" t="s">
         <v>29</v>
@@ -3979,7 +3983,7 @@
         <v>37</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P34" s="1" t="s">
         <v>179</v>
@@ -3988,7 +3992,7 @@
         <v>28</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S34" s="1" t="s">
         <v>29</v>
@@ -4032,7 +4036,7 @@
         <v>28</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S35" s="1" t="s">
         <v>29</v>
@@ -4055,7 +4059,7 @@
         <v>92</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>22</v>
@@ -4070,7 +4074,7 @@
         <v>32</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P36" s="1" t="s">
         <v>187</v>
@@ -4079,7 +4083,7 @@
         <v>28</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S36" s="1" t="s">
         <v>29</v>
@@ -4096,7 +4100,7 @@
         <v>32</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>189</v>
@@ -4126,7 +4130,7 @@
         <v>22</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S37" s="1" t="s">
         <v>29</v>
@@ -4146,7 +4150,7 @@
         <v>37</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>194</v>
@@ -4176,7 +4180,7 @@
         <v>28</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S38" s="1" t="s">
         <v>29</v>
@@ -4217,7 +4221,7 @@
         <v>33</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P39" s="1" t="s">
         <v>203</v>
@@ -4226,7 +4230,7 @@
         <v>22</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S39" s="1" t="s">
         <v>29</v>
@@ -4276,7 +4280,7 @@
         <v>22</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S40" s="1" t="s">
         <v>29</v>
@@ -4296,7 +4300,7 @@
         <v>68</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>210</v>
@@ -4317,7 +4321,7 @@
         <v>68</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P41" s="1" t="s">
         <v>212</v>
@@ -4326,7 +4330,7 @@
         <v>43</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S41" s="1" t="s">
         <v>29</v>
@@ -4346,7 +4350,7 @@
         <v>37</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>214</v>
@@ -4355,7 +4359,7 @@
         <v>22</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>215</v>
@@ -4370,16 +4374,16 @@
         <v>216</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q42" s="1" t="s">
         <v>43</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S42" s="1" t="s">
         <v>29</v>
@@ -4399,7 +4403,7 @@
         <v>37</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>218</v>
@@ -4420,7 +4424,7 @@
         <v>68</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P43" s="1" t="s">
         <v>220</v>
@@ -4429,7 +4433,7 @@
         <v>22</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S43" s="1" t="s">
         <v>29</v>
@@ -4449,7 +4453,7 @@
         <v>101</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>222</v>
@@ -4458,7 +4462,7 @@
         <v>22</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>223</v>
@@ -4473,7 +4477,7 @@
         <v>68</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P44" s="1" t="s">
         <v>224</v>
@@ -4482,7 +4486,7 @@
         <v>22</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S44" s="1" t="s">
         <v>29</v>
@@ -4502,7 +4506,7 @@
         <v>37</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>226</v>
@@ -4523,7 +4527,7 @@
         <v>37</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P45" s="1" t="s">
         <v>228</v>
@@ -4532,7 +4536,7 @@
         <v>28</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S45" s="1" t="s">
         <v>29</v>
@@ -4552,7 +4556,7 @@
         <v>68</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>230</v>
@@ -4573,7 +4577,7 @@
         <v>33</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P46" s="1" t="s">
         <v>232</v>
@@ -4582,13 +4586,13 @@
         <v>28</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S46" s="1" t="s">
         <v>29</v>
       </c>
       <c r="U46" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="60" x14ac:dyDescent="0.25">
@@ -4635,7 +4639,7 @@
         <v>43</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S47" s="1" t="s">
         <v>29</v>
@@ -4655,7 +4659,7 @@
         <v>239</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>240</v>
@@ -4685,7 +4689,7 @@
         <v>28</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S48" s="1" t="s">
         <v>29</v>
@@ -4705,7 +4709,7 @@
         <v>33</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>244</v>
@@ -4714,7 +4718,7 @@
         <v>28</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>245</v>
@@ -4729,7 +4733,7 @@
         <v>33</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P49" s="1" t="s">
         <v>246</v>
@@ -4738,7 +4742,7 @@
         <v>28</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S49" s="1" t="s">
         <v>29</v>
@@ -4758,7 +4762,7 @@
         <v>248</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>249</v>
@@ -4788,7 +4792,7 @@
         <v>28</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S50" s="1" t="s">
         <v>29</v>
@@ -4808,7 +4812,7 @@
         <v>33</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>253</v>
@@ -4829,7 +4833,7 @@
         <v>255</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P51" s="1" t="s">
         <v>256</v>
@@ -4838,7 +4842,7 @@
         <v>22</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S51" s="1" t="s">
         <v>29</v>
@@ -4879,7 +4883,7 @@
         <v>33</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P52" s="1" t="s">
         <v>260</v>
@@ -4888,7 +4892,7 @@
         <v>22</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S52" s="1" t="s">
         <v>29</v>
@@ -4929,7 +4933,7 @@
         <v>264</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P53" s="1" t="s">
         <v>265</v>
@@ -4938,7 +4942,7 @@
         <v>22</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S53" s="1" t="s">
         <v>29</v>
@@ -4958,7 +4962,7 @@
         <v>267</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>268</v>
@@ -4979,7 +4983,7 @@
         <v>37</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P54" s="1" t="s">
         <v>270</v>
@@ -4988,7 +4992,7 @@
         <v>22</v>
       </c>
       <c r="R54" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S54" s="1" t="s">
         <v>29</v>
@@ -5008,7 +5012,7 @@
         <v>196</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>272</v>
@@ -5017,7 +5021,7 @@
         <v>22</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>273</v>
@@ -5032,7 +5036,7 @@
         <v>196</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="P55" s="1" t="s">
         <v>274</v>
@@ -5041,7 +5045,7 @@
         <v>28</v>
       </c>
       <c r="R55" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S55" s="1" t="s">
         <v>29</v>
@@ -5071,24 +5075,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5096,10 +5100,10 @@
         <v>108</v>
       </c>
       <c r="B4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" t="s">
         <v>324</v>
-      </c>
-      <c r="C4" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5107,21 +5111,21 @@
         <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B6" t="s">
         <v>332</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>333</v>
-      </c>
-      <c r="C6" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5129,10 +5133,10 @@
         <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5140,10 +5144,10 @@
         <v>219</v>
       </c>
       <c r="B8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C8" t="s">
         <v>369</v>
-      </c>
-      <c r="C8" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5151,10 +5155,10 @@
         <v>221</v>
       </c>
       <c r="B9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5162,10 +5166,10 @@
         <v>225</v>
       </c>
       <c r="B10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5173,10 +5177,10 @@
         <v>227</v>
       </c>
       <c r="B11" t="s">
+        <v>374</v>
+      </c>
+      <c r="C11" t="s">
         <v>375</v>
-      </c>
-      <c r="C11" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5184,32 +5188,32 @@
         <v>229</v>
       </c>
       <c r="B12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>366</v>
+      </c>
+      <c r="B15" t="s">
         <v>367</v>
       </c>
-      <c r="B15" t="s">
-        <v>368</v>
-      </c>
       <c r="C15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5217,10 +5221,10 @@
         <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5228,10 +5232,10 @@
         <v>193</v>
       </c>
       <c r="B18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5239,18 +5243,18 @@
         <v>215</v>
       </c>
       <c r="B20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>334</v>
+      </c>
+      <c r="B21" t="s">
         <v>335</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>336</v>
-      </c>
-      <c r="C21" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5258,10 +5262,10 @@
         <v>211</v>
       </c>
       <c r="B22" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5269,10 +5273,10 @@
         <v>163</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C23" t="s">
         <v>350</v>
-      </c>
-      <c r="C23" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5280,10 +5284,10 @@
         <v>164</v>
       </c>
       <c r="B24" t="s">
+        <v>351</v>
+      </c>
+      <c r="C24" t="s">
         <v>352</v>
-      </c>
-      <c r="C24" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5291,21 +5295,21 @@
         <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -5313,10 +5317,10 @@
         <v>154</v>
       </c>
       <c r="B28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5324,10 +5328,10 @@
         <v>170</v>
       </c>
       <c r="B29" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C29" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5335,21 +5339,21 @@
         <v>269</v>
       </c>
       <c r="B30" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>304</v>
+      </c>
+      <c r="B32" t="s">
         <v>305</v>
       </c>
-      <c r="B32" t="s">
-        <v>306</v>
-      </c>
       <c r="C32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5357,10 +5361,10 @@
         <v>105</v>
       </c>
       <c r="B33" t="s">
+        <v>321</v>
+      </c>
+      <c r="C33" t="s">
         <v>322</v>
-      </c>
-      <c r="C33" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5368,10 +5372,10 @@
         <v>178</v>
       </c>
       <c r="B34" t="s">
+        <v>357</v>
+      </c>
+      <c r="C34" t="s">
         <v>358</v>
-      </c>
-      <c r="C34" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -5379,57 +5383,57 @@
         <v>152</v>
       </c>
       <c r="B36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C36" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>325</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>327</v>
-      </c>
       <c r="C37" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>302</v>
+      </c>
+      <c r="B38" t="s">
+        <v>307</v>
+      </c>
+      <c r="C38" t="s">
         <v>303</v>
-      </c>
-      <c r="B38" t="s">
-        <v>308</v>
-      </c>
-      <c r="C38" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>313</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>315</v>
-      </c>
       <c r="C39" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>297</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>299</v>
-      </c>
       <c r="C40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -5437,10 +5441,10 @@
         <v>223</v>
       </c>
       <c r="B41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C41" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -5448,10 +5452,10 @@
         <v>266</v>
       </c>
       <c r="B42" t="s">
+        <v>377</v>
+      </c>
+      <c r="C42" t="s">
         <v>378</v>
-      </c>
-      <c r="C42" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -5459,10 +5463,10 @@
         <v>118</v>
       </c>
       <c r="B43" t="s">
+        <v>327</v>
+      </c>
+      <c r="C43" t="s">
         <v>328</v>
-      </c>
-      <c r="C43" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -5470,10 +5474,10 @@
         <v>156</v>
       </c>
       <c r="B44" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C44" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -5481,10 +5485,10 @@
         <v>121</v>
       </c>
       <c r="B45" t="s">
+        <v>329</v>
+      </c>
+      <c r="C45" t="s">
         <v>330</v>
-      </c>
-      <c r="C45" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -5492,10 +5496,10 @@
         <v>172</v>
       </c>
       <c r="B46" t="s">
+        <v>355</v>
+      </c>
+      <c r="C46" t="s">
         <v>356</v>
-      </c>
-      <c r="C46" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -5503,32 +5507,32 @@
         <v>78</v>
       </c>
       <c r="B48" t="s">
+        <v>311</v>
+      </c>
+      <c r="C48" t="s">
         <v>312</v>
-      </c>
-      <c r="C48" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C49" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>308</v>
+      </c>
+      <c r="B50" t="s">
         <v>309</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>310</v>
-      </c>
-      <c r="C50" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5536,10 +5540,10 @@
         <v>159</v>
       </c>
       <c r="B51" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C51" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5547,21 +5551,21 @@
         <v>168</v>
       </c>
       <c r="B53" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C53" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5569,10 +5573,10 @@
         <v>213</v>
       </c>
       <c r="B55" t="s">
+        <v>362</v>
+      </c>
+      <c r="C55" t="s">
         <v>363</v>
-      </c>
-      <c r="C55" t="s">
-        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaks I guess? I don't remember how I edited these files but probably some typo fixes I made and forgot to commit/push 2 weeks ago
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_1_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_1_CC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11167F8-2EF4-4D29-932D-1E0326DBD69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED8F3C3-3FA4-468B-8214-6B5E218B5A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,24 @@
     <sheet name="Tactile Tabletop Data - Level 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="411">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -1254,6 +1266,12 @@
   </si>
   <si>
     <t>character's that are bad for squib: new lines,the dot dot dot single character,</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Tier</t>
   </si>
 </sst>
 </file>
@@ -2114,2940 +2132,3326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W55"/>
+  <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="33.140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="44.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="43.42578125" customWidth="1"/>
-    <col min="23" max="16384" width="22.28515625" style="1"/>
+    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="33.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="44.42578125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="43.42578125" customWidth="1"/>
+    <col min="25" max="16384" width="22.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <f>ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <f>ROW()-1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:B55" si="0">ROW()-1</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:25" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:25" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:25" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="U13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="W14" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="U15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="U16" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="T19" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="U19" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="U20" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="S21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="U21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="W21" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S22" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="S23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R23" s="1" t="s">
+      <c r="T23" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="U23" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="M24" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="Q24" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="R24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R24" s="1" t="s">
+      <c r="T24" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S24" s="1" t="s">
+      <c r="U24" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="M25" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="S25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="U25" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="S26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S26" s="1" t="s">
+      <c r="U26" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M27" s="1" t="s">
+      <c r="N27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="S27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S27" s="1" t="s">
+      <c r="U27" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="M28" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="L28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M28" s="1" t="s">
+      <c r="N28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="R28" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="S28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="U28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="P29" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="S29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="U29" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="M30" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M30" s="1" t="s">
+      <c r="N30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="S30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R30" s="1" t="s">
+      <c r="T30" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="U30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U30" s="1" t="s">
+      <c r="W30" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="M31" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M31" s="1" t="s">
+      <c r="N31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="S31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R31" s="1" t="s">
+      <c r="T31" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S31" s="1" t="s">
+      <c r="U31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M32" s="1" t="s">
+      <c r="N32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="S32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R32" s="1" t="s">
+      <c r="T32" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S32" s="1" t="s">
+      <c r="U32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="M33" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M33" s="1" t="s">
+      <c r="N33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P33" s="1" t="s">
+      <c r="R33" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="S33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R33" s="1" t="s">
+      <c r="T33" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S33" s="1" t="s">
+      <c r="U33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="M34" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M34" s="1" t="s">
+      <c r="N34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="Q34" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P34" s="1" t="s">
+      <c r="R34" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R34" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S34" s="1" t="s">
+      <c r="U34" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="M35" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="Q35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="R35" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="S35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="U35" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="M36" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P36" s="1" t="s">
+      <c r="R36" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="S36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="U36" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="M37" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="P37" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P37" s="1" t="s">
+      <c r="R37" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="S37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R37" s="1" t="s">
+      <c r="T37" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S37" s="1" t="s">
+      <c r="U37" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="M38" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="P38" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="O38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="R38" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="S38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="U38" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="39" spans="1:23" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="P39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O39" s="1" t="s">
+      <c r="Q39" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="R39" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="Q39" s="1" t="s">
+      <c r="S39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R39" s="1" t="s">
+      <c r="T39" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S39" s="1" t="s">
+      <c r="U39" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="M40" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M40" s="1" t="s">
+      <c r="N40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="P40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="Q40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="R40" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="S40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R40" s="1" t="s">
+      <c r="T40" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="U40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="41" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>1</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K41" s="2" t="s">
+      <c r="M41" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M41" s="1" t="s">
+      <c r="N41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O41" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="P41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O41" s="1" t="s">
+      <c r="Q41" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P41" s="1" t="s">
+      <c r="R41" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="Q41" s="1" t="s">
+      <c r="S41" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R41" s="1" t="s">
+      <c r="T41" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S41" s="1" t="s">
+      <c r="U41" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="42" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>1</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="M42" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M42" s="1" t="s">
+      <c r="N42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="P42" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="O42" s="1" t="s">
+      <c r="Q42" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P42" s="1" t="s">
+      <c r="R42" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="Q42" s="1" t="s">
+      <c r="S42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R42" s="1" t="s">
+      <c r="T42" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S42" s="1" t="s">
+      <c r="U42" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="43" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K43" s="2" t="s">
+      <c r="M43" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M43" s="1" t="s">
+      <c r="N43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O43" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="P43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O43" s="1" t="s">
+      <c r="Q43" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P43" s="1" t="s">
+      <c r="R43" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="Q43" s="1" t="s">
+      <c r="S43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R43" s="1" t="s">
+      <c r="T43" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S43" s="1" t="s">
+      <c r="U43" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>1</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="M44" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="L44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="P44" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O44" s="1" t="s">
+      <c r="Q44" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P44" s="1" t="s">
+      <c r="R44" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="Q44" s="1" t="s">
+      <c r="S44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R44" s="1" t="s">
+      <c r="T44" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S44" s="1" t="s">
+      <c r="U44" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="45" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="M45" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M45" s="1" t="s">
+      <c r="N45" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N45" s="1" t="s">
+      <c r="P45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O45" s="1" t="s">
+      <c r="Q45" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P45" s="1" t="s">
+      <c r="R45" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="Q45" s="1" t="s">
+      <c r="S45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R45" s="1" t="s">
+      <c r="T45" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S45" s="1" t="s">
+      <c r="U45" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+    <row r="46" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="M46" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N46" s="1" t="s">
+      <c r="P46" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O46" s="1" t="s">
+      <c r="Q46" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P46" s="1" t="s">
+      <c r="R46" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="Q46" s="1" t="s">
+      <c r="S46" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R46" s="1" t="s">
+      <c r="T46" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S46" s="1" t="s">
+      <c r="U46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U46" s="1" t="s">
+      <c r="W46" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="47" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="M47" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="L47" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M47" s="1" t="s">
+      <c r="N47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O47" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N47" s="1" t="s">
+      <c r="P47" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O47" s="1" t="s">
+      <c r="Q47" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P47" s="1" t="s">
+      <c r="R47" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="Q47" s="1" t="s">
+      <c r="S47" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S47" s="1" t="s">
+      <c r="U47" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="M48" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M48" s="1" t="s">
+      <c r="N48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O48" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N48" s="1" t="s">
+      <c r="P48" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="Q48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P48" s="1" t="s">
+      <c r="R48" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="Q48" s="1" t="s">
+      <c r="S48" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R48" s="1" t="s">
+      <c r="T48" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S48" s="1" t="s">
+      <c r="U48" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="49" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>1</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="M49" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="N49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="O49" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N49" s="1" t="s">
+      <c r="P49" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O49" s="1" t="s">
+      <c r="Q49" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P49" s="1" t="s">
+      <c r="R49" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="Q49" s="1" t="s">
+      <c r="S49" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R49" s="1" t="s">
+      <c r="T49" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="U49" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="90" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="50" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>1</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="M50" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="L50" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M50" s="1" t="s">
+      <c r="N50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O50" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N50" s="1" t="s">
+      <c r="P50" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O50" s="1" t="s">
+      <c r="Q50" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P50" s="1" t="s">
+      <c r="R50" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="Q50" s="1" t="s">
+      <c r="S50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R50" s="1" t="s">
+      <c r="T50" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S50" s="1" t="s">
+      <c r="U50" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="51" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>1</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="M51" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M51" s="1" t="s">
+      <c r="N51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O51" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N51" s="1" t="s">
+      <c r="P51" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="O51" s="1" t="s">
+      <c r="Q51" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P51" s="1" t="s">
+      <c r="R51" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="Q51" s="1" t="s">
+      <c r="S51" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R51" s="1" t="s">
+      <c r="T51" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S51" s="1" t="s">
+      <c r="U51" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="52" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>1</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K52" s="2" t="s">
+      <c r="M52" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="L52" s="1" t="s">
+      <c r="N52" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M52" s="1" t="s">
+      <c r="O52" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N52" s="1" t="s">
+      <c r="P52" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O52" s="1" t="s">
+      <c r="Q52" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P52" s="1" t="s">
+      <c r="R52" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="Q52" s="1" t="s">
+      <c r="S52" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R52" s="1" t="s">
+      <c r="T52" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S52" s="1" t="s">
+      <c r="U52" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>1</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="M53" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="L53" s="1" t="s">
+      <c r="N53" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M53" s="1" t="s">
+      <c r="O53" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N53" s="1" t="s">
+      <c r="P53" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="O53" s="1" t="s">
+      <c r="Q53" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P53" s="1" t="s">
+      <c r="R53" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="Q53" s="1" t="s">
+      <c r="S53" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R53" s="1" t="s">
+      <c r="T53" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S53" s="1" t="s">
+      <c r="U53" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="54" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="M54" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="L54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M54" s="1" t="s">
+      <c r="N54" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O54" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N54" s="1" t="s">
+      <c r="P54" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O54" s="1" t="s">
+      <c r="Q54" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="P54" s="1" t="s">
+      <c r="R54" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="Q54" s="1" t="s">
+      <c r="S54" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R54" s="1" t="s">
+      <c r="T54" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S54" s="1" t="s">
+      <c r="U54" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>1</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="K55" s="2" t="s">
+      <c r="M55" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="L55" s="1" t="s">
+      <c r="N55" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M55" s="1" t="s">
+      <c r="O55" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N55" s="1" t="s">
+      <c r="P55" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="O55" s="1" t="s">
+      <c r="Q55" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P55" s="1" t="s">
+      <c r="R55" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="Q55" s="1" t="s">
+      <c r="S55" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R55" s="1" t="s">
+      <c r="T55" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="S55" s="1" t="s">
+      <c r="U55" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>